<commit_message>
Almost finishing data cleaning
</commit_message>
<xml_diff>
--- a/Projects/LendingClubProject/dict/LendingClubDataDictionary.xlsx
+++ b/Projects/LendingClubProject/dict/LendingClubDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nleea\Desktop\daiy\Learning\RoadToHokage\Knowledge\Knowledge\DataScience\Projects\LendingClubProject\dict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FDD111-D22E-462A-922E-6FABCEAE3318}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E64E60-3908-4005-BCBD-A5C8C4A6AD2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-870" yWindow="4070" windowWidth="16590" windowHeight="9040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -2288,7 +2288,7 @@
   </sheetPr>
   <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A91" sqref="A91"/>
     </sheetView>
@@ -3609,9 +3609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>